<commit_message>
minor modification in input data
</commit_message>
<xml_diff>
--- a/Two node models/in.xlsx
+++ b/Two node models/in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Locational-investment-signals\Two node models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA9F5CBE-8AE2-4A4B-8565-A4E14169C1D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7CB3299-83C6-4A6D-9FCC-4F7FBCE6BA87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1955,52 +1955,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>14924.7</c:v>
+                  <c:v>14379.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14587.7</c:v>
+                  <c:v>13789.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15045.9</c:v>
+                  <c:v>14153.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16594.599999999999</c:v>
+                  <c:v>17161.900000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>18776.7</c:v>
+                  <c:v>18808.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20142.400000000001</c:v>
+                  <c:v>21544.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20846.900000000001</c:v>
+                  <c:v>22245.1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>21167.8</c:v>
+                  <c:v>20230.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20634.900000000001</c:v>
+                  <c:v>21542.799999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20019.5</c:v>
+                  <c:v>19811.900000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>19793.400000000001</c:v>
+                  <c:v>18444.900000000001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20247.5</c:v>
+                  <c:v>19799.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20080.900000000001</c:v>
+                  <c:v>19702.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>18874.3</c:v>
+                  <c:v>19641.099999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17420.900000000001</c:v>
+                  <c:v>16586.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15876.5</c:v>
+                  <c:v>15000.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2101,52 +2101,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>29849.5</c:v>
+                  <c:v>30394.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>29175.4</c:v>
+                  <c:v>29973.200000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>30091.9</c:v>
+                  <c:v>30983.9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>33189.199999999997</c:v>
+                  <c:v>32621.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37553.300000000003</c:v>
+                  <c:v>37521.699999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40284.800000000003</c:v>
+                  <c:v>38882.300000000003</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41693.9</c:v>
+                  <c:v>40295.699999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42335.7</c:v>
+                  <c:v>43272.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41269.699999999997</c:v>
+                  <c:v>40361.800000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40039</c:v>
+                  <c:v>40246.699999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>39586.699999999997</c:v>
+                  <c:v>40935.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40495</c:v>
+                  <c:v>40942.9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40161.800000000003</c:v>
+                  <c:v>40540.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>37748.6</c:v>
+                  <c:v>36981.800000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34841.800000000003</c:v>
+                  <c:v>35676.300000000003</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>31753.1</c:v>
+                  <c:v>32629.200000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4833,8 +4833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BF2839-4BDE-4B18-A7A4-A5F1FDEE19B7}">
   <dimension ref="A1:Y95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4907,10 +4907,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>14924.7</v>
+        <v>14379.6</v>
       </c>
       <c r="D4">
-        <v>29849.5</v>
+        <v>30394.6</v>
       </c>
       <c r="E4" s="45">
         <v>1</v>
@@ -4936,10 +4936,10 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>14587.7</v>
+        <v>13789.9</v>
       </c>
       <c r="D5">
-        <v>29175.4</v>
+        <v>29973.200000000001</v>
       </c>
       <c r="E5" s="45">
         <v>2</v>
@@ -4969,10 +4969,10 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>15045.9</v>
+        <v>14153.9</v>
       </c>
       <c r="D6">
-        <v>30091.9</v>
+        <v>30983.9</v>
       </c>
       <c r="E6" s="45">
         <v>3</v>
@@ -5002,10 +5002,10 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>16594.599999999999</v>
+        <v>17161.900000000001</v>
       </c>
       <c r="D7">
-        <v>33189.199999999997</v>
+        <v>32621.9</v>
       </c>
       <c r="E7" s="45">
         <v>4</v>
@@ -5035,10 +5035,10 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>18776.7</v>
+        <v>18808.2</v>
       </c>
       <c r="D8">
-        <v>37553.300000000003</v>
+        <v>37521.699999999997</v>
       </c>
       <c r="E8" s="45">
         <v>5</v>
@@ -5068,10 +5068,10 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>20142.400000000001</v>
+        <v>21544.9</v>
       </c>
       <c r="D9">
-        <v>40284.800000000003</v>
+        <v>38882.300000000003</v>
       </c>
       <c r="E9" s="45">
         <v>6</v>
@@ -5101,10 +5101,10 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>20846.900000000001</v>
+        <v>22245.1</v>
       </c>
       <c r="D10">
-        <v>41693.9</v>
+        <v>40295.699999999997</v>
       </c>
       <c r="E10" s="45">
         <v>7</v>
@@ -5134,10 +5134,10 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>21167.8</v>
+        <v>20230.8</v>
       </c>
       <c r="D11">
-        <v>42335.7</v>
+        <v>43272.7</v>
       </c>
       <c r="E11" s="45">
         <v>8</v>
@@ -5167,10 +5167,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>20634.900000000001</v>
+        <v>21542.799999999999</v>
       </c>
       <c r="D12">
-        <v>41269.699999999997</v>
+        <v>40361.800000000003</v>
       </c>
       <c r="E12" s="45">
         <v>9</v>
@@ -5200,10 +5200,10 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>20019.5</v>
+        <v>19811.900000000001</v>
       </c>
       <c r="D13">
-        <v>40039</v>
+        <v>40246.699999999997</v>
       </c>
       <c r="E13" s="45">
         <v>10</v>
@@ -5233,10 +5233,10 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <v>19793.400000000001</v>
+        <v>18444.900000000001</v>
       </c>
       <c r="D14">
-        <v>39586.699999999997</v>
+        <v>40935.199999999997</v>
       </c>
       <c r="E14" s="45">
         <v>11</v>
@@ -5266,10 +5266,10 @@
         <v>12</v>
       </c>
       <c r="C15">
-        <v>20247.5</v>
+        <v>19799.5</v>
       </c>
       <c r="D15">
-        <v>40495</v>
+        <v>40942.9</v>
       </c>
       <c r="E15" s="45">
         <v>12</v>
@@ -5299,10 +5299,10 @@
         <v>13</v>
       </c>
       <c r="C16">
-        <v>20080.900000000001</v>
+        <v>19702.599999999999</v>
       </c>
       <c r="D16">
-        <v>40161.800000000003</v>
+        <v>40540.199999999997</v>
       </c>
       <c r="E16" s="45">
         <v>13</v>
@@ -5332,10 +5332,10 @@
         <v>14</v>
       </c>
       <c r="C17">
-        <v>18874.3</v>
+        <v>19641.099999999999</v>
       </c>
       <c r="D17">
-        <v>37748.6</v>
+        <v>36981.800000000003</v>
       </c>
       <c r="E17" s="45">
         <v>14</v>
@@ -5365,10 +5365,10 @@
         <v>15</v>
       </c>
       <c r="C18">
-        <v>17420.900000000001</v>
+        <v>16586.3</v>
       </c>
       <c r="D18">
-        <v>34841.800000000003</v>
+        <v>35676.300000000003</v>
       </c>
       <c r="E18" s="45">
         <v>15</v>
@@ -5398,10 +5398,10 @@
         <v>16</v>
       </c>
       <c r="C19">
-        <v>15876.5</v>
+        <v>15000.4</v>
       </c>
       <c r="D19">
-        <v>31753.1</v>
+        <v>32629.200000000001</v>
       </c>
       <c r="E19" s="45">
         <v>16</v>

</xml_diff>

<commit_message>
input data 12 h
</commit_message>
<xml_diff>
--- a/Two node models/in.xlsx
+++ b/Two node models/in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Locational-investment-signals\Two node models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C27B1940-BF2D-4035-8BD8-4D4BF60DA09F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4323277F-D80A-49B7-9FC1-21219A7969C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>Availability</t>
   </si>
@@ -215,12 +215,6 @@
   </si>
   <si>
     <t>16:30-18:00</t>
-  </si>
-  <si>
-    <t>18:00-19:30</t>
-  </si>
-  <si>
-    <t>19:30-21:00</t>
   </si>
   <si>
     <t>Soll</t>
@@ -1311,46 +1305,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>0.48499999999999999</c:v>
+                  <c:v>0.43333333333333302</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.30499999999999999</c:v>
+                  <c:v>0.245</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.19500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.20499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.105</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16999999999999901</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0.22</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.18</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.06</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.105</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.16999999999999901</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.22</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.26500000000000001</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.27500000000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.21</c:v>
+                  <c:v>0.17499999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1401,42 +1389,36 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.06</c:v>
+                  <c:v>0.19500000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.315</c:v>
+                  <c:v>0.35499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.09</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>1.4999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.315</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.105</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.4999999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.19</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.32</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.24</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1485,46 +1467,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="23"/>
                 <c:pt idx="0">
-                  <c:v>0.32999999999999902</c:v>
+                  <c:v>0.30666666666666598</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.22</c:v>
+                  <c:v>0.16499999999999901</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.13500000000000001</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.11499999999999901</c:v>
+                  <c:v>0.14499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>0.08</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4999999999999895E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.245</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.20499999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.13</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.08</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8.4999999999999895E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.21</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.29499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.30499999999999999</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.12</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1575,42 +1551,36 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.01</c:v>
+                  <c:v>8.4999999999999895E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.23499999999999999</c:v>
+                  <c:v>0.30499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.20499999999999999</c:v>
+                  <c:v>9.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>0.02</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.29499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.44500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.26500000000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.02</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.29499999999999998</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.45</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.41</c:v>
-                </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.4999999999999997E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1898,7 +1868,7 @@
             <c:strRef>
               <c:f>timeseries!$A$4:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0:00-1:30</c:v>
                 </c:pt>
@@ -1934,12 +1904,6 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>16:30-18:00</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>18:00-19:30</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>19:30-21:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1951,46 +1915,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>16298.88</c:v>
+                  <c:v>15928.06</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18204.96</c:v>
+                  <c:v>21328.264999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21940.264999999999</c:v>
+                  <c:v>21434.51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>22432.76</c:v>
+                  <c:v>24612.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24780.9</c:v>
+                  <c:v>20955.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20955.12</c:v>
+                  <c:v>18520.035</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>18520.035</c:v>
+                  <c:v>19324.22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19324.22</c:v>
+                  <c:v>25682.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>25682.75</c:v>
+                  <c:v>22480.240000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23438.240000000002</c:v>
+                  <c:v>20161.71</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20418.27</c:v>
+                  <c:v>18851.23</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20428.72</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>16306.32</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>15532.8</c:v>
+                  <c:v>15145.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2032,7 +1990,7 @@
             <c:strRef>
               <c:f>timeseries!$A$4:$A$19</c:f>
               <c:strCache>
-                <c:ptCount val="14"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0:00-1:30</c:v>
                 </c:pt>
@@ -2068,12 +2026,6 @@
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>16:30-18:00</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>18:00-19:30</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>19:30-21:00</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2085,46 +2037,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>35445.119999999901</c:v>
+                  <c:v>37316.606666666601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45290.54</c:v>
+                  <c:v>50997.735000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52425.735000000001</c:v>
+                  <c:v>52444.99</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>48954.239999999998</c:v>
+                  <c:v>46750.05</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48104.1</c:v>
+                  <c:v>45755.88</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>45755.88</c:v>
+                  <c:v>33724.964999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33724.964999999997</c:v>
+                  <c:v>34640.78</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>34640.78</c:v>
+                  <c:v>41926.25</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41926.25</c:v>
+                  <c:v>45616.2599999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>45497.7599999999</c:v>
+                  <c:v>43860.789999999899</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>45400.729999999901</c:v>
+                  <c:v>40958.769999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42416.28</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>37088.18</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>36243.199999999997</c:v>
+                  <c:v>35339.85</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4812,7 +4758,7 @@
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:I17"/>
+      <selection activeCell="F4" sqref="F4:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4885,22 +4831,22 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>16298.88</v>
+        <v>15928.06</v>
       </c>
       <c r="D4">
-        <v>35445.119999999901</v>
+        <v>37316.606666666601</v>
       </c>
       <c r="E4" s="45">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>0.48499999999999999</v>
+        <v>0.43333333333333302</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
       <c r="H4">
-        <v>0.32999999999999902</v>
+        <v>0.30666666666666598</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -4914,25 +4860,25 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>18204.96</v>
+        <v>21328.264999999999</v>
       </c>
       <c r="D5">
-        <v>45290.54</v>
+        <v>50997.735000000001</v>
       </c>
       <c r="E5" s="45">
         <v>2</v>
       </c>
       <c r="F5">
-        <v>0.30499999999999999</v>
+        <v>0.245</v>
       </c>
       <c r="G5">
-        <v>0.06</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="H5">
-        <v>0.22</v>
+        <v>0.16499999999999901</v>
       </c>
       <c r="I5">
-        <v>0.01</v>
+        <v>8.4999999999999895E-2</v>
       </c>
       <c r="V5" s="56"/>
       <c r="W5" s="57"/>
@@ -4947,10 +4893,10 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>21940.264999999999</v>
+        <v>21434.51</v>
       </c>
       <c r="D6">
-        <v>52425.735000000001</v>
+        <v>52444.99</v>
       </c>
       <c r="E6" s="45">
         <v>3</v>
@@ -4959,13 +4905,13 @@
         <v>0.19500000000000001</v>
       </c>
       <c r="G6">
-        <v>0.315</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="H6">
-        <v>0.13500000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="I6">
-        <v>0.23499999999999999</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="V6" s="59"/>
       <c r="W6" s="60"/>
@@ -4980,25 +4926,25 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>22432.76</v>
+        <v>24612.45</v>
       </c>
       <c r="D7">
-        <v>48954.239999999998</v>
+        <v>46750.05</v>
       </c>
       <c r="E7" s="45">
         <v>4</v>
       </c>
       <c r="F7">
-        <v>0.22</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="G7">
-        <v>0.31</v>
+        <v>0.18</v>
       </c>
       <c r="H7">
-        <v>0.11499999999999901</v>
+        <v>0.14499999999999999</v>
       </c>
       <c r="I7">
-        <v>0.20499999999999999</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="V7" s="59"/>
       <c r="W7" s="60"/>
@@ -5013,25 +4959,25 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>24780.9</v>
+        <v>20955.12</v>
       </c>
       <c r="D8">
-        <v>48104.1</v>
+        <v>45755.88</v>
       </c>
       <c r="E8" s="45">
         <v>5</v>
       </c>
       <c r="F8">
-        <v>0.18</v>
+        <v>0.125</v>
       </c>
       <c r="G8">
-        <v>0.09</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0.14000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="I8">
-        <v>7.0000000000000007E-2</v>
+        <v>0</v>
       </c>
       <c r="V8" s="59"/>
       <c r="W8" s="60"/>
@@ -5046,22 +4992,22 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>20955.12</v>
+        <v>18520.035</v>
       </c>
       <c r="D9">
-        <v>45755.88</v>
+        <v>33724.964999999997</v>
       </c>
       <c r="E9" s="45">
         <v>6</v>
       </c>
       <c r="F9">
-        <v>0.125</v>
+        <v>0.06</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
       <c r="H9">
-        <v>0.13</v>
+        <v>0.08</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -5079,25 +5025,25 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>18520.035</v>
+        <v>19324.22</v>
       </c>
       <c r="D10">
-        <v>33724.964999999997</v>
+        <v>34640.78</v>
       </c>
       <c r="E10" s="45">
         <v>7</v>
       </c>
       <c r="F10">
-        <v>0.06</v>
+        <v>0.105</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="H10">
-        <v>0.08</v>
+        <v>8.4999999999999895E-2</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="V10" s="59"/>
       <c r="W10" s="60"/>
@@ -5112,25 +5058,25 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>19324.22</v>
+        <v>25682.75</v>
       </c>
       <c r="D11">
-        <v>34640.78</v>
+        <v>41926.25</v>
       </c>
       <c r="E11" s="45">
         <v>8</v>
       </c>
       <c r="F11">
-        <v>0.105</v>
+        <v>0.16999999999999901</v>
       </c>
       <c r="G11">
-        <v>1.4999999999999999E-2</v>
+        <v>0.19</v>
       </c>
       <c r="H11">
-        <v>8.4999999999999895E-2</v>
+        <v>0.16</v>
       </c>
       <c r="I11">
-        <v>0.02</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="V11" s="59"/>
       <c r="W11" s="60"/>
@@ -5145,25 +5091,25 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>25682.75</v>
+        <v>22480.240000000002</v>
       </c>
       <c r="D12">
-        <v>41926.25</v>
+        <v>45616.2599999999</v>
       </c>
       <c r="E12" s="45">
         <v>9</v>
       </c>
       <c r="F12">
-        <v>0.16999999999999901</v>
+        <v>0.23499999999999999</v>
       </c>
       <c r="G12">
-        <v>0.19</v>
+        <v>0.315</v>
       </c>
       <c r="H12">
-        <v>0.16</v>
+        <v>0.245</v>
       </c>
       <c r="I12">
-        <v>0.29499999999999998</v>
+        <v>0.44500000000000001</v>
       </c>
       <c r="V12" s="59"/>
       <c r="W12" s="60"/>
@@ -5178,25 +5124,25 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>23438.240000000002</v>
+        <v>20161.71</v>
       </c>
       <c r="D13">
-        <v>45497.7599999999</v>
+        <v>43860.789999999899</v>
       </c>
       <c r="E13" s="45">
         <v>10</v>
       </c>
       <c r="F13">
-        <v>0.22</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="G13">
+        <v>0.105</v>
+      </c>
+      <c r="H13">
         <v>0.32</v>
       </c>
-      <c r="H13">
-        <v>0.21</v>
-      </c>
       <c r="I13">
-        <v>0.45</v>
+        <v>0.26500000000000001</v>
       </c>
       <c r="V13" s="59"/>
       <c r="W13" s="60"/>
@@ -5211,25 +5157,25 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <v>20418.27</v>
+        <v>18851.23</v>
       </c>
       <c r="D14">
-        <v>45400.729999999901</v>
+        <v>40958.769999999997</v>
       </c>
       <c r="E14" s="45">
         <v>11</v>
       </c>
       <c r="F14">
-        <v>0.26500000000000001</v>
+        <v>0.22</v>
       </c>
       <c r="G14">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="H14">
-        <v>0.29499999999999998</v>
+        <v>0.20499999999999999</v>
       </c>
       <c r="I14">
-        <v>0.41</v>
+        <v>0</v>
       </c>
       <c r="V14" s="59"/>
       <c r="W14" s="60"/>
@@ -5244,25 +5190,25 @@
         <v>12</v>
       </c>
       <c r="C15">
-        <v>20428.72</v>
+        <v>15145.65</v>
       </c>
       <c r="D15">
-        <v>42416.28</v>
+        <v>35339.85</v>
       </c>
       <c r="E15" s="45">
         <v>12</v>
       </c>
       <c r="F15">
-        <v>0.27500000000000002</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="G15">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H15">
-        <v>0.30499999999999999</v>
+        <v>0.13</v>
       </c>
       <c r="I15">
-        <v>7.4999999999999997E-2</v>
+        <v>0</v>
       </c>
       <c r="V15" s="59"/>
       <c r="W15" s="60"/>
@@ -5270,72 +5216,30 @@
       <c r="Y15" s="60"/>
     </row>
     <row r="16" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="45">
-        <v>13</v>
-      </c>
-      <c r="C16">
-        <v>16306.32</v>
-      </c>
-      <c r="D16">
-        <v>37088.18</v>
-      </c>
-      <c r="E16" s="45">
-        <v>13</v>
-      </c>
-      <c r="F16">
-        <v>0.16</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0.12</v>
-      </c>
-      <c r="I16">
-        <v>0</v>
-      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
       <c r="V16" s="59"/>
       <c r="W16" s="60"/>
       <c r="X16" s="61"/>
       <c r="Y16" s="60"/>
     </row>
-    <row r="17" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="45">
-        <v>14</v>
-      </c>
-      <c r="C17">
-        <v>15532.8</v>
-      </c>
-      <c r="D17">
-        <v>36243.199999999997</v>
-      </c>
-      <c r="E17" s="45">
-        <v>14</v>
-      </c>
-      <c r="F17">
-        <v>0.21</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0.15</v>
-      </c>
-      <c r="I17">
-        <v>0</v>
-      </c>
+    <row r="17" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
       <c r="V17" s="59"/>
       <c r="W17" s="60"/>
       <c r="X17" s="61"/>
       <c r="Y17" s="60"/>
     </row>
-    <row r="18" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
       <c r="V18" s="59"/>
@@ -5343,7 +5247,7 @@
       <c r="X18" s="61"/>
       <c r="Y18" s="60"/>
     </row>
-    <row r="19" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
       <c r="V19" s="59"/>
@@ -5351,13 +5255,13 @@
       <c r="X19" s="61"/>
       <c r="Y19" s="60"/>
     </row>
-    <row r="20" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="V20" s="59"/>
       <c r="W20" s="60"/>
       <c r="X20" s="61"/>
       <c r="Y20" s="60"/>
     </row>
-    <row r="21" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
       <c r="V21" s="59"/>
@@ -5365,19 +5269,19 @@
       <c r="X21" s="61"/>
       <c r="Y21" s="60"/>
     </row>
-    <row r="22" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="V22" s="59"/>
       <c r="W22" s="60"/>
       <c r="X22" s="61"/>
       <c r="Y22" s="60"/>
     </row>
-    <row r="23" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="V23" s="59"/>
       <c r="W23" s="60"/>
       <c r="X23" s="61"/>
       <c r="Y23" s="60"/>
     </row>
-    <row r="24" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>
       <c r="V24" s="59"/>
@@ -5385,19 +5289,19 @@
       <c r="X24" s="61"/>
       <c r="Y24" s="60"/>
     </row>
-    <row r="25" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="V25" s="59"/>
       <c r="W25" s="60"/>
       <c r="X25" s="61"/>
       <c r="Y25" s="60"/>
     </row>
-    <row r="26" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="V26" s="59"/>
       <c r="W26" s="60"/>
       <c r="X26" s="61"/>
       <c r="Y26" s="60"/>
     </row>
-    <row r="27" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C27" s="47"/>
       <c r="D27" s="47"/>
       <c r="V27" s="59"/>
@@ -5405,7 +5309,7 @@
       <c r="X27" s="61"/>
       <c r="Y27" s="60"/>
     </row>
-    <row r="28" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="3:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C28" s="47"/>
       <c r="D28" s="47"/>
       <c r="V28" s="59"/>
@@ -5413,19 +5317,19 @@
       <c r="X28" s="61"/>
       <c r="Y28" s="60"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="29" spans="3:25" x14ac:dyDescent="0.35">
       <c r="C29" s="47"/>
       <c r="D29" s="47"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="30" spans="3:25" x14ac:dyDescent="0.35">
       <c r="C30" s="47"/>
       <c r="D30" s="47"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="31" spans="3:25" x14ac:dyDescent="0.35">
       <c r="C31" s="47"/>
       <c r="D31" s="47"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="32" spans="3:25" x14ac:dyDescent="0.35">
       <c r="C32" s="47"/>
       <c r="D32" s="47"/>
     </row>
@@ -5451,11 +5355,11 @@
       </c>
       <c r="M35" s="47">
         <f>N43</f>
-        <v>1861.4999999999995</v>
+        <v>1790.9333333333325</v>
       </c>
       <c r="N35" s="47">
         <f>P43</f>
-        <v>1548.6428571428557</v>
+        <v>1512.3166666666655</v>
       </c>
     </row>
     <row r="36" spans="3:17" x14ac:dyDescent="0.35">
@@ -5466,11 +5370,11 @@
       </c>
       <c r="M36" s="47">
         <f>O43</f>
-        <v>976.11428571428576</v>
+        <v>989.15</v>
       </c>
       <c r="N36" s="47">
         <f>Q43</f>
-        <v>1107.5142857142857</v>
+        <v>1102.3</v>
       </c>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.35">
@@ -5529,19 +5433,19 @@
       </c>
       <c r="N43" s="51">
         <f>(8760*N44)</f>
-        <v>1861.4999999999995</v>
+        <v>1790.9333333333325</v>
       </c>
       <c r="O43" s="51">
         <f t="shared" ref="O43:Q43" si="0">(8760*O44)</f>
-        <v>976.11428571428576</v>
+        <v>989.15</v>
       </c>
       <c r="P43" s="51">
         <f t="shared" si="0"/>
-        <v>1548.6428571428557</v>
+        <v>1512.3166666666655</v>
       </c>
       <c r="Q43" s="51">
         <f t="shared" si="0"/>
-        <v>1107.5142857142857</v>
+        <v>1102.3</v>
       </c>
     </row>
     <row r="44" spans="3:17" x14ac:dyDescent="0.35">
@@ -5552,26 +5456,26 @@
       </c>
       <c r="N44" s="52">
         <f>AVERAGE(F4:F26)</f>
-        <v>0.21249999999999994</v>
+        <v>0.20444444444444435</v>
       </c>
       <c r="O44" s="52">
         <f>AVERAGE(G4:G26)</f>
-        <v>0.11142857142857143</v>
+        <v>0.11291666666666667</v>
       </c>
       <c r="P44" s="52">
         <f>AVERAGE(H4:H26)</f>
-        <v>0.17678571428571413</v>
+        <v>0.17263888888888876</v>
       </c>
       <c r="Q44" s="52">
         <f>AVERAGE(I4:I26)</f>
-        <v>0.12642857142857142</v>
+        <v>0.12583333333333332</v>
       </c>
     </row>
     <row r="45" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C45" s="47"/>
       <c r="D45" s="47"/>
       <c r="L45" s="45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N45" s="45">
         <v>21</v>

</xml_diff>

<commit_message>
new input data with more distinct load profiles
</commit_message>
<xml_diff>
--- a/Two node models/in.xlsx
+++ b/Two node models/in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Locational-investment-signals\Two node models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4323277F-D80A-49B7-9FC1-21219A7969C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC29D8F3-A065-40AB-B77C-81CFBC5868AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1915,40 +1915,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>15928.06</c:v>
+                  <c:v>12728.1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21328.264999999999</c:v>
+                  <c:v>14509.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21434.51</c:v>
+                  <c:v>15966.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24612.45</c:v>
+                  <c:v>22739.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20955.12</c:v>
+                  <c:v>19954.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18520.035</c:v>
+                  <c:v>21614.9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>19324.22</c:v>
+                  <c:v>18904.599999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25682.75</c:v>
+                  <c:v>15283.9</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>22480.240000000002</c:v>
+                  <c:v>24613.9</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20161.71</c:v>
+                  <c:v>19174.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>18851.23</c:v>
+                  <c:v>14419.5</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>15145.65</c:v>
+                  <c:v>15409.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2037,40 +2037,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>37316.606666666601</c:v>
+                  <c:v>31989.3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50997.735000000001</c:v>
+                  <c:v>41208.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52444.99</c:v>
+                  <c:v>46824</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46750.05</c:v>
+                  <c:v>37273.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45755.88</c:v>
+                  <c:v>39508.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>33724.964999999997</c:v>
+                  <c:v>29103.4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34640.78</c:v>
+                  <c:v>25812.799999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>41926.25</c:v>
+                  <c:v>40433.800000000003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>45616.2599999999</c:v>
+                  <c:v>38176.699999999997</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>43860.789999999899</c:v>
+                  <c:v>40838.400000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40958.769999999997</c:v>
+                  <c:v>45043.199999999997</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>35339.85</c:v>
+                  <c:v>35308.400000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4758,7 +4758,7 @@
   <dimension ref="A1:Y95"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:I15"/>
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4831,10 +4831,10 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>15928.06</v>
+        <v>12728.1</v>
       </c>
       <c r="D4">
-        <v>37316.606666666601</v>
+        <v>31989.3</v>
       </c>
       <c r="E4" s="45">
         <v>1</v>
@@ -4860,10 +4860,10 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>21328.264999999999</v>
+        <v>14509.7</v>
       </c>
       <c r="D5">
-        <v>50997.735000000001</v>
+        <v>41208.1</v>
       </c>
       <c r="E5" s="45">
         <v>2</v>
@@ -4893,10 +4893,10 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>21434.51</v>
+        <v>15966.6</v>
       </c>
       <c r="D6">
-        <v>52444.99</v>
+        <v>46824</v>
       </c>
       <c r="E6" s="45">
         <v>3</v>
@@ -4926,10 +4926,10 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>24612.45</v>
+        <v>22739.5</v>
       </c>
       <c r="D7">
-        <v>46750.05</v>
+        <v>37273.199999999997</v>
       </c>
       <c r="E7" s="45">
         <v>4</v>
@@ -4959,10 +4959,10 @@
         <v>5</v>
       </c>
       <c r="C8">
-        <v>20955.12</v>
+        <v>19954.2</v>
       </c>
       <c r="D8">
-        <v>45755.88</v>
+        <v>39508.5</v>
       </c>
       <c r="E8" s="45">
         <v>5</v>
@@ -4992,10 +4992,10 @@
         <v>6</v>
       </c>
       <c r="C9">
-        <v>18520.035</v>
+        <v>21614.9</v>
       </c>
       <c r="D9">
-        <v>33724.964999999997</v>
+        <v>29103.4</v>
       </c>
       <c r="E9" s="45">
         <v>6</v>
@@ -5025,10 +5025,10 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <v>19324.22</v>
+        <v>18904.599999999999</v>
       </c>
       <c r="D10">
-        <v>34640.78</v>
+        <v>25812.799999999999</v>
       </c>
       <c r="E10" s="45">
         <v>7</v>
@@ -5058,10 +5058,10 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>25682.75</v>
+        <v>15283.9</v>
       </c>
       <c r="D11">
-        <v>41926.25</v>
+        <v>40433.800000000003</v>
       </c>
       <c r="E11" s="45">
         <v>8</v>
@@ -5091,10 +5091,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>22480.240000000002</v>
+        <v>24613.9</v>
       </c>
       <c r="D12">
-        <v>45616.2599999999</v>
+        <v>38176.699999999997</v>
       </c>
       <c r="E12" s="45">
         <v>9</v>
@@ -5124,10 +5124,10 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>20161.71</v>
+        <v>19174.3</v>
       </c>
       <c r="D13">
-        <v>43860.789999999899</v>
+        <v>40838.400000000001</v>
       </c>
       <c r="E13" s="45">
         <v>10</v>
@@ -5157,10 +5157,10 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <v>18851.23</v>
+        <v>14419.5</v>
       </c>
       <c r="D14">
-        <v>40958.769999999997</v>
+        <v>45043.199999999997</v>
       </c>
       <c r="E14" s="45">
         <v>11</v>
@@ -5190,10 +5190,10 @@
         <v>12</v>
       </c>
       <c r="C15">
-        <v>15145.65</v>
+        <v>15409.9</v>
       </c>
       <c r="D15">
-        <v>35339.85</v>
+        <v>35308.400000000001</v>
       </c>
       <c r="E15" s="45">
         <v>12</v>

</xml_diff>

<commit_message>
first results for the updated input data
</commit_message>
<xml_diff>
--- a/Two node models/in.xlsx
+++ b/Two node models/in.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Locational-investment-signals\Two node models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.eicke\Documents\Locational-investment-signals\Two node models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC29D8F3-A065-40AB-B77C-81CFBC5868AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677D732B-954E-443C-88E2-1E908BCB1FEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cost" sheetId="2" r:id="rId1"/>
@@ -117,107 +117,107 @@
     <t>south</t>
   </si>
   <si>
+    <t>in %</t>
+  </si>
+  <si>
+    <t>Cost of transmission extension</t>
+  </si>
+  <si>
+    <t>Cost for Südlink (€)</t>
+  </si>
+  <si>
+    <t>Length of Südlink (km)</t>
+  </si>
+  <si>
+    <t>Capacity of Südlink (MW)</t>
+  </si>
+  <si>
+    <t>Cost (€/MW)</t>
+  </si>
+  <si>
+    <t>Lifetime (y)</t>
+  </si>
+  <si>
+    <t>Annulized costs</t>
+  </si>
+  <si>
+    <t>Additional costs in southern region</t>
+  </si>
+  <si>
+    <t>cost_add_var_s</t>
+  </si>
+  <si>
+    <t>cost_add_fix_s</t>
+  </si>
+  <si>
+    <t>CPF</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>peak</t>
+  </si>
+  <si>
+    <t>200€ per km per year</t>
+  </si>
+  <si>
+    <t>in MW</t>
+  </si>
+  <si>
+    <t>Wind</t>
+  </si>
+  <si>
+    <t>Solar</t>
+  </si>
+  <si>
+    <t>North</t>
+  </si>
+  <si>
+    <t>South</t>
+  </si>
+  <si>
+    <t>0:00-1:30</t>
+  </si>
+  <si>
+    <t>1:30-3:00</t>
+  </si>
+  <si>
+    <t>3:00-4:30</t>
+  </si>
+  <si>
+    <t>4:30-6:00</t>
+  </si>
+  <si>
+    <t>6:00-7:30</t>
+  </si>
+  <si>
+    <t>7:30-9:00</t>
+  </si>
+  <si>
+    <t>9:00-10:30</t>
+  </si>
+  <si>
+    <t>10:30-12:00</t>
+  </si>
+  <si>
+    <t>12:00-13:30</t>
+  </si>
+  <si>
+    <t>13:30-15:00</t>
+  </si>
+  <si>
+    <t>15:00-16:30</t>
+  </si>
+  <si>
+    <t>16:30-18:00</t>
+  </si>
+  <si>
+    <t>Soll</t>
+  </si>
+  <si>
     <t>AFC
-(€/kW)</t>
-  </si>
-  <si>
-    <t>in %</t>
-  </si>
-  <si>
-    <t>Cost of transmission extension</t>
-  </si>
-  <si>
-    <t>Cost for Südlink (€)</t>
-  </si>
-  <si>
-    <t>Length of Südlink (km)</t>
-  </si>
-  <si>
-    <t>Capacity of Südlink (MW)</t>
-  </si>
-  <si>
-    <t>Cost (€/MW)</t>
-  </si>
-  <si>
-    <t>Lifetime (y)</t>
-  </si>
-  <si>
-    <t>Annulized costs</t>
-  </si>
-  <si>
-    <t>Additional costs in southern region</t>
-  </si>
-  <si>
-    <t>cost_add_var_s</t>
-  </si>
-  <si>
-    <t>cost_add_fix_s</t>
-  </si>
-  <si>
-    <t>CPF</t>
-  </si>
-  <si>
-    <t>base</t>
-  </si>
-  <si>
-    <t>peak</t>
-  </si>
-  <si>
-    <t>200€ per km per year</t>
-  </si>
-  <si>
-    <t>in MW</t>
-  </si>
-  <si>
-    <t>Wind</t>
-  </si>
-  <si>
-    <t>Solar</t>
-  </si>
-  <si>
-    <t>North</t>
-  </si>
-  <si>
-    <t>South</t>
-  </si>
-  <si>
-    <t>0:00-1:30</t>
-  </si>
-  <si>
-    <t>1:30-3:00</t>
-  </si>
-  <si>
-    <t>3:00-4:30</t>
-  </si>
-  <si>
-    <t>4:30-6:00</t>
-  </si>
-  <si>
-    <t>6:00-7:30</t>
-  </si>
-  <si>
-    <t>7:30-9:00</t>
-  </si>
-  <si>
-    <t>9:00-10:30</t>
-  </si>
-  <si>
-    <t>10:30-12:00</t>
-  </si>
-  <si>
-    <t>12:00-13:30</t>
-  </si>
-  <si>
-    <t>13:30-15:00</t>
-  </si>
-  <si>
-    <t>15:00-16:30</t>
-  </si>
-  <si>
-    <t>16:30-18:00</t>
-  </si>
-  <si>
-    <t>Soll</t>
+(€/kW p.a.)</t>
   </si>
 </sst>
 </file>
@@ -815,7 +815,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -964,10 +964,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>95</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>603.07999999999993</c:v>
+                  <c:v>630.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,10 +1027,10 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>40</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>679.48</c:v>
+                  <c:v>679.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1096,7 +1096,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="589632111"/>
@@ -1156,7 +1156,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="589627951"/>
@@ -1197,7 +1197,7 @@
       <a:pPr>
         <a:defRPr sz="1100"/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1249,7 +1249,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1646,7 +1646,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="509294543"/>
@@ -1705,7 +1705,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="509296207"/>
@@ -1747,7 +1747,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1777,7 +1777,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1828,7 +1828,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2135,7 +2135,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="509307439"/>
@@ -2194,7 +2194,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-DE"/>
+            <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="509309103"/>
@@ -2236,7 +2236,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-DE"/>
+          <a:endParaRPr lang="de-DE"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2266,7 +2266,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-DE"/>
+      <a:endParaRPr lang="de-DE"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4368,8 +4368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4431,14 +4431,14 @@
         <v>11</v>
       </c>
       <c r="G3" s="20" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="H3" s="39" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -4463,10 +4463,10 @@
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -4482,7 +4482,7 @@
     </row>
     <row r="5" spans="1:16" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="7">
         <v>2000</v>
@@ -4497,26 +4497,26 @@
         <v>0.32</v>
       </c>
       <c r="G5" s="42">
-        <v>95</v>
+        <v>280</v>
       </c>
       <c r="H5" s="40">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="N5" s="28" t="s">
         <v>13</v>
       </c>
       <c r="O5" s="12">
         <f>G5</f>
-        <v>95</v>
+        <v>280</v>
       </c>
       <c r="P5" s="13">
         <f t="shared" ref="P5" si="0">G5+H5*$P$4/1000</f>
-        <v>603.07999999999993</v>
+        <v>630.4</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="7">
         <v>1700</v>
@@ -4531,21 +4531,21 @@
         <v>0.27</v>
       </c>
       <c r="G6" s="42">
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="H6" s="40">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="N6" s="28" t="s">
         <v>14</v>
       </c>
       <c r="O6" s="14">
         <f>G6</f>
-        <v>40</v>
+        <v>110</v>
       </c>
       <c r="P6" s="15">
         <f>G6+H6*$P$4/1000</f>
-        <v>679.48</v>
+        <v>679.4</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="16.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -4565,7 +4565,7 @@
         <v>0</v>
       </c>
       <c r="G7" s="42">
-        <v>80</v>
+        <v>100</v>
       </c>
       <c r="H7" s="40">
         <f>E7/D7+F7/D7*$C$33</f>
@@ -4591,7 +4591,7 @@
       <c r="E8" s="9"/>
       <c r="F8" s="10"/>
       <c r="G8" s="42">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="H8" s="40">
         <v>0</v>
@@ -4667,12 +4667,12 @@
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="11">
         <f>10000000000</f>
@@ -4681,7 +4681,7 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="11">
         <v>700</v>
@@ -4689,7 +4689,7 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="11">
         <v>4000</v>
@@ -4701,7 +4701,7 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" s="44">
         <f>C37/C39</f>
@@ -4713,7 +4713,7 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C42" s="11">
         <v>40</v>
@@ -4724,7 +4724,7 @@
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C44" s="11">
         <f>C41*$C$30*(1+$C$30)^C42/((1+$C$30)^C42-1)</f>
@@ -4739,7 +4739,7 @@
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.35">
       <c r="C47" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -4757,8 +4757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58BF2839-4BDE-4B18-A7A4-A5F1FDEE19B7}">
   <dimension ref="A1:Y95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4770,12 +4770,12 @@
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="C1" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="66"/>
       <c r="E1" s="46"/>
       <c r="F1" s="66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G1" s="66"/>
       <c r="H1" s="66"/>
@@ -4825,7 +4825,7 @@
     </row>
     <row r="4" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="45" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B4" s="45">
         <v>1</v>
@@ -4854,7 +4854,7 @@
     </row>
     <row r="5" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" s="45">
         <v>2</v>
@@ -4887,7 +4887,7 @@
     </row>
     <row r="6" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="45" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="45">
         <v>3</v>
@@ -4920,7 +4920,7 @@
     </row>
     <row r="7" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="45">
         <v>4</v>
@@ -4953,7 +4953,7 @@
     </row>
     <row r="8" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="45" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="45">
         <v>5</v>
@@ -4986,7 +4986,7 @@
     </row>
     <row r="9" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="45" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="45">
         <v>6</v>
@@ -5019,7 +5019,7 @@
     </row>
     <row r="10" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="45">
         <v>7</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="11" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="45">
         <v>8</v>
@@ -5085,7 +5085,7 @@
     </row>
     <row r="12" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="45" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="45">
         <v>9</v>
@@ -5118,7 +5118,7 @@
     </row>
     <row r="13" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="45">
         <v>10</v>
@@ -5151,7 +5151,7 @@
     </row>
     <row r="14" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="45">
         <v>11</v>
@@ -5184,7 +5184,7 @@
     </row>
     <row r="15" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="45">
         <v>12</v>
@@ -5341,17 +5341,17 @@
       <c r="C34" s="47"/>
       <c r="D34" s="47"/>
       <c r="M34" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="N34" s="45" t="s">
         <v>46</v>
-      </c>
-      <c r="N34" s="45" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="35" spans="3:17" x14ac:dyDescent="0.35">
       <c r="C35" s="47"/>
       <c r="D35" s="47"/>
       <c r="L35" s="45" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M35" s="47">
         <f>N43</f>
@@ -5366,7 +5366,7 @@
       <c r="C36" s="47"/>
       <c r="D36" s="47"/>
       <c r="L36" s="45" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M36" s="47">
         <f>O43</f>
@@ -5452,7 +5452,7 @@
       <c r="C44" s="47"/>
       <c r="D44" s="47"/>
       <c r="L44" s="46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N44" s="52">
         <f>AVERAGE(F4:F26)</f>
@@ -5475,7 +5475,7 @@
       <c r="C45" s="47"/>
       <c r="D45" s="47"/>
       <c r="L45" s="45" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N45" s="45">
         <v>21</v>

</xml_diff>